<commit_message>
Correção do campo pesquisa em Usuarios e filmes
</commit_message>
<xml_diff>
--- a/webroot/relatorios/Relatorio.xlsx
+++ b/webroot/relatorios/Relatorio.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Codigo Reserva</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>2021-10-29T13:11:18-03:00</t>
+  </si>
+  <si>
+    <t>2021-11-16T21:56:50-03:00</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,6 +640,23 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>5.6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção do campo pesquisa em Clientes e Reservas, adição de JS no dropdown
</commit_message>
<xml_diff>
--- a/webroot/relatorios/Relatorio.xlsx
+++ b/webroot/relatorios/Relatorio.xlsx
@@ -15,84 +15,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
-  <si>
-    <t>Codigo Reserva</t>
-  </si>
-  <si>
-    <t>Data de Entrada do Valor</t>
-  </si>
-  <si>
-    <t>Valor Total Pago</t>
-  </si>
-  <si>
-    <t>Filme</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+  <si>
+    <t>Código Reserva</t>
+  </si>
+  <si>
+    <t>Valor Multa</t>
+  </si>
+  <si>
+    <t>Data de Devolução</t>
+  </si>
+  <si>
+    <t>Data lime de Devolução</t>
   </si>
   <si>
     <t>Cliente</t>
   </si>
   <si>
-    <t>2021-10-22T12:02:18-03:00</t>
-  </si>
-  <si>
-    <t>Homem de Ferro 1</t>
+    <t>2021-10-29T13:11:13-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T13:55:00-03:00</t>
   </si>
   <si>
     <t>Jose Gabriel Batista Machado</t>
   </si>
   <si>
-    <t>2021-10-22T12:02:33-03:00</t>
-  </si>
-  <si>
-    <t>Star Wars: The Clone Wars</t>
+    <t>2021-10-29T13:11:18-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T14:21:00-03:00</t>
   </si>
   <si>
     <t>Murilo jose</t>
   </si>
   <si>
-    <t>2021-10-22T14:17:36-03:00</t>
-  </si>
-  <si>
-    <t>O incrível Hulk</t>
-  </si>
-  <si>
-    <t>2021-10-22T14:40:58-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-22T16:26:04-03:00</t>
-  </si>
-  <si>
-    <t>Rei Arthur</t>
-  </si>
-  <si>
-    <t>Isaque Almeida Damascen</t>
-  </si>
-  <si>
     <t>2021-10-25T14:25:27-03:00</t>
   </si>
   <si>
-    <t>2021-10-26T10:45:31-03:00</t>
-  </si>
-  <si>
-    <t>A Culpa e das Estrelas</t>
+    <t>2021-10-26T16:54:24-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T14:31:00-03:00</t>
   </si>
   <si>
     <t>Flavia Cristina nascimento</t>
   </si>
   <si>
-    <t>2021-10-26T16:54:24-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-29T13:09:11-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-29T13:11:13-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-29T13:11:18-03:00</t>
-  </si>
-  <si>
     <t>2021-11-16T21:56:50-03:00</t>
+  </si>
+  <si>
+    <t>2021-11-16T11:49:00-03:00</t>
   </si>
 </sst>
 </file>
@@ -431,7 +404,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,13 +431,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>3.75</v>
+      <c r="B2">
+        <v>33.4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -475,13 +448,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>33.2</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3">
-        <v>3.6</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -492,171 +465,52 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>21.6</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>3.6</v>
-      </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>3.75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>2.85</v>
-      </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>25.35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>2.55</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>8.6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
-        <v>0.15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11">
-        <v>37.15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12">
-        <v>36.8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>5.6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>